<commit_message>
End of task update
</commit_message>
<xml_diff>
--- a/NLRepairSpecs.xlsx
+++ b/NLRepairSpecs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nordic\Projets\ProgramationDivers\NordicLamSplitAnalysis\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nordic\Projets\ProgramationDivers\NordicLamSplitAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE3C645-1B40-4340-B417-46B4D3739742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AE5EA7-EA13-4FD2-AD74-313F54B504D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="1095" windowWidth="16440" windowHeight="27825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16080" yWindow="8460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NordicLamSpecs" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Name\label</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>NRes</t>
+  </si>
+  <si>
+    <t>PLPremium</t>
   </si>
 </sst>
 </file>
@@ -946,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,63 +1208,70 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="I11" s="2">
-        <v>71</v>
-      </c>
+      <c r="G11" s="2">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="H11">
+        <v>0.8</v>
+      </c>
+      <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="I12" s="2">
+        <v>71</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2">
+      <c r="F13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
         <v>619</v>
       </c>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1280,6 +1290,14 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="119" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>